<commit_message>
Managed devices samples updated
</commit_message>
<xml_diff>
--- a/Samples/Intune-Managed-devices.xlsx
+++ b/Samples/Intune-Managed-devices.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toni\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFSRepo\atwork\D365-Manual-Reports\Manual\Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EA90E0-0B34-44E0-BDA3-E948E2B498E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63EE025-222E-44C9-AEE3-8FD775C52847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="1875" windowWidth="22905" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1875" windowWidth="22905" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Managed devices" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
   <si>
     <t>OU</t>
   </si>
@@ -151,7 +151,7 @@
     <t>PartnerReportedThreatState</t>
   </si>
   <si>
-    <t>no data available</t>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -544,9 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -729,6 +727,132 @@
       <c r="A2" t="s">
         <v>43</v>
       </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>